<commit_message>
New output per Excel file
</commit_message>
<xml_diff>
--- a/zib2017-2020/mapping/excel/MedicatieToediening2.xlsx
+++ b/zib2017-2020/mapping/excel/MedicatieToediening2.xlsx
@@ -1,20 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marcd\Dropbox\development\Zibtranslate\zib2017-2020\mapping\excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F60354A1-17DD-4331-AFA0-82DA9D4CC2EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="MedicatieToediening" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="70">
   <si>
     <t>ZibName</t>
   </si>
@@ -61,17 +80,176 @@
     <t>TRANSLATIE_spec_terug</t>
   </si>
   <si>
+    <t>Medicatieafspraak</t>
+  </si>
+  <si>
+    <t>ZIB-911</t>
+  </si>
+  <si>
+    <t>In engelse vertaling overal Farmaceutical vervangen door Pharmaceutical (7X)</t>
+  </si>
+  <si>
+    <t>CONCEPT NAME CHANGED (EN)</t>
+  </si>
+  <si>
+    <t>Toelichting</t>
+  </si>
+  <si>
+    <t>low</t>
+  </si>
+  <si>
+    <t>Toedieningsafspraak</t>
+  </si>
+  <si>
+    <t>oranje: minor</t>
+  </si>
+  <si>
+    <t>groen: geen wijzigingen</t>
+  </si>
+  <si>
+    <t>MedicatieToediening</t>
+  </si>
+  <si>
+    <t>NL-CM:9.13.20928</t>
+  </si>
+  <si>
+    <t>ToedieningsProduct::FarmaceutischProduct</t>
+  </si>
+  <si>
+    <t>NL-CM:9.13.20929</t>
+  </si>
+  <si>
+    <t>Toedieningssnelheid::Bereik</t>
+  </si>
+  <si>
+    <t>NL-CM:9.13.23159</t>
+  </si>
+  <si>
+    <t>ToedieningsDatumTijd</t>
+  </si>
+  <si>
+    <t>NL-CM:9.13.21193</t>
+  </si>
+  <si>
+    <t>AfgesprokenDatumTijd</t>
+  </si>
+  <si>
+    <t>NL-CM:9.13.23171</t>
+  </si>
+  <si>
+    <t>ToegediendeHoeveelheid</t>
+  </si>
+  <si>
+    <t>NL-CM:9.13.21194</t>
+  </si>
+  <si>
+    <t>AfwijkendeToediening</t>
+  </si>
+  <si>
+    <t>NL-CM:9.13.23167</t>
+  </si>
+  <si>
+    <t>Toedieningsweg</t>
+  </si>
+  <si>
+    <t>NL-CM:9.13.21195</t>
+  </si>
+  <si>
+    <t>MedicatieToedieningToedieningswegCodelijst</t>
+  </si>
+  <si>
+    <t>DubbeleControleUitgevoerd</t>
+  </si>
+  <si>
+    <t>NL-CM:9.13.23168</t>
+  </si>
+  <si>
+    <t>NL-CM:9.13.23170</t>
+  </si>
+  <si>
+    <t>NL-CM:9.13.23237</t>
+  </si>
+  <si>
+    <t>GerelateerdeAfspraak</t>
+  </si>
+  <si>
+    <t>NL-CM:9.13.23169</t>
+  </si>
+  <si>
+    <t>Toediener</t>
+  </si>
+  <si>
+    <t>NL-CM:9.13.21196</t>
+  </si>
+  <si>
+    <t>Patiënt</t>
+  </si>
+  <si>
+    <t>NL-CM:9.13.23380</t>
+  </si>
+  <si>
+    <t>Zorgverlener</t>
+  </si>
+  <si>
+    <t>NL-CM:9.13.23172</t>
+  </si>
+  <si>
+    <t>Mantelzorger::Contactpersoon</t>
+  </si>
+  <si>
+    <t>NL-CM:9.13.23355</t>
+  </si>
+  <si>
+    <t>MedicatieToedieningRedenVanAfwijken</t>
+  </si>
+  <si>
+    <t>NL-CM:9.13.23166</t>
+  </si>
+  <si>
+    <t>MedicatieToedieningRedenVanAfwijkenCodelijst</t>
+  </si>
+  <si>
+    <t>MedicatieToedieningStatus</t>
+  </si>
+  <si>
+    <t>NL-CM:9.13.21191</t>
+  </si>
+  <si>
+    <t>MedicatieToedieningStatusCodelijst</t>
+  </si>
+  <si>
+    <t>NL-CM:9.13.21337</t>
+  </si>
+  <si>
+    <t>ZIB-812</t>
+  </si>
+  <si>
+    <t>Kardinaliteit van element 'ToegediendeHoeveelheid'  gewijzigd van 1 naar 0..1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONCEPT NAME CHANGED (EN): AgreedMedicine::FarmaceuticalProduct -&gt; AgreedMedicine::PharmaceuticalProduct </t>
+  </si>
+  <si>
+    <t>CONCEPT NAME CHANGED (EN): AgreedMedicine::PharmaceuticalProduct -&gt; AgreedMedicine::FarmaceuticalProduct</t>
+  </si>
+  <si>
+    <t>ONE TO ZERO-TO-ONE</t>
+  </si>
+  <si>
+    <t>ZERO-TO-ONE TO ONE</t>
+  </si>
+  <si>
+    <t>CARDINALITY CHANGE</t>
+  </si>
+  <si>
     <t>MedicatieToediening2</t>
-  </si>
-  <si>
-    <t>Medicatie zibs momenteel on hold</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -87,16 +265,41 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -111,36 +314,273 @@
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="19">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6857A58F-37AF-0844-853C-D07449BEE558}" name="Table1" displayName="Table1" ref="A1:O20" totalsRowShown="0" headerRowDxfId="18" dataDxfId="16" headerRowBorderDxfId="17" tableBorderDxfId="15">
+  <autoFilter ref="A1:O20" xr:uid="{6857A58F-37AF-0844-853C-D07449BEE558}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O14">
+    <sortCondition ref="D2:D14"/>
+  </sortState>
+  <tableColumns count="15">
+    <tableColumn id="1" xr3:uid="{1A7B4B02-112E-B545-A552-8EFBCF17B8F7}" name="ZibName" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{50B22E84-DC1B-6E47-8E2E-B827113AD00A}" name="ConceptID_2017" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{078FCA97-2D35-0244-9213-F29E12CB197F}" name="ConceptName_2017" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{EB7E0D71-BAEF-A047-A851-746ADD0F48F6}" name="Codelists_2017" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{EE9120CB-50C1-4E42-AFD5-D6389532D5DA}" name="Change" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{C4B60B25-3DDB-184C-97E2-9C2E1D317EC0}" name="ConceptID_2020" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{FE8D53A8-93D9-8541-A509-555AB95DFFBF}" name="ConceptName_2020" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{39BD8A52-445D-9C4A-BD8C-30FED6FA9DEF}" name="Codelists_2020" dataDxfId="7"/>
+    <tableColumn id="9" xr3:uid="{59C4E602-55C0-6E49-ABB7-9A263CC3EE22}" name="Bits" dataDxfId="6"/>
+    <tableColumn id="10" xr3:uid="{4E61526F-6862-AA46-A432-F85E4A10F6BD}" name="Omschrijving" dataDxfId="5"/>
+    <tableColumn id="11" xr3:uid="{A4CD3601-98A8-594E-A455-E4A735344D40}" name="TypeChange" dataDxfId="4"/>
+    <tableColumn id="12" xr3:uid="{8B9CCC28-2BCA-EB4F-9B33-C32B554EE625}" name="Impact_heen" dataDxfId="3"/>
+    <tableColumn id="13" xr3:uid="{19A0AD34-1030-0F46-B7ED-AFAEAEED001C}" name="TRANSLATIE_spec_heen" dataDxfId="2"/>
+    <tableColumn id="14" xr3:uid="{C83F05E2-32D1-1F4B-8137-355EE865E389}" name="Impact_terug" dataDxfId="1"/>
+    <tableColumn id="15" xr3:uid="{BC09DA06-2792-4742-81C9-AE6522EB0978}" name="TRANSLATIE_spec_terug" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -178,7 +618,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -212,6 +652,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -246,9 +687,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -421,14 +863,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:O39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A20"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="3" max="3" width="35.85546875" customWidth="1"/>
+    <col min="4" max="4" width="68.42578125" customWidth="1"/>
+    <col min="5" max="5" width="29.85546875" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" customWidth="1"/>
+    <col min="7" max="7" width="40.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="37.140625" customWidth="1"/>
+    <col min="10" max="10" width="54.28515625" customWidth="1"/>
+    <col min="11" max="11" width="27.140625" customWidth="1"/>
+    <col min="12" max="12" width="40.28515625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="33.7109375" customWidth="1"/>
+    <col min="14" max="14" width="25.7109375" style="2" customWidth="1"/>
+    <col min="15" max="15" width="31.7109375" style="2" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -462,31 +922,547 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2"/>
+      <c r="M2" s="2"/>
+      <c r="N2"/>
+    </row>
+    <row r="3" spans="1:15" ht="75" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="N3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" t="s">
+        <v>28</v>
+      </c>
+      <c r="K4" s="2"/>
+      <c r="L4"/>
+      <c r="M4" s="2"/>
+      <c r="N4"/>
+    </row>
+    <row r="5" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" t="s">
+        <v>30</v>
+      </c>
+      <c r="L5"/>
+      <c r="N5"/>
+    </row>
+    <row r="6" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" t="s">
+        <v>32</v>
+      </c>
+      <c r="L6"/>
+      <c r="N6"/>
+    </row>
+    <row r="7" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I7" t="s">
+        <v>62</v>
+      </c>
+      <c r="J7" t="s">
+        <v>63</v>
+      </c>
+      <c r="K7" t="s">
+        <v>68</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M7" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O7" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G8" t="s">
+        <v>36</v>
+      </c>
+      <c r="L8"/>
+      <c r="M8" s="2"/>
+      <c r="N8"/>
+    </row>
+    <row r="9" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9" t="s">
+        <v>38</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="K9" s="2"/>
+      <c r="L9"/>
+      <c r="M9" s="2"/>
+      <c r="N9"/>
+    </row>
+    <row r="10" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>69</v>
+      </c>
+      <c r="B10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10" t="s">
+        <v>41</v>
+      </c>
+      <c r="H10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10"/>
+      <c r="M10" s="2"/>
+      <c r="N10"/>
+    </row>
+    <row r="11" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" t="s">
         <v>15</v>
       </c>
-      <c r="B2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" t="s">
-        <v>16</v>
-      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G11" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" s="2"/>
+      <c r="L11"/>
+      <c r="M11" s="2"/>
+      <c r="N11"/>
+    </row>
+    <row r="12" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>69</v>
+      </c>
+      <c r="B12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G12" t="s">
+        <v>21</v>
+      </c>
+      <c r="H12" s="2"/>
+      <c r="L12"/>
+      <c r="M12" s="2"/>
+      <c r="N12"/>
+    </row>
+    <row r="13" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>69</v>
+      </c>
+      <c r="B13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G13" t="s">
+        <v>45</v>
+      </c>
+      <c r="H13" s="2"/>
+      <c r="L13"/>
+      <c r="N13"/>
+    </row>
+    <row r="14" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>69</v>
+      </c>
+      <c r="B14" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G14" t="s">
+        <v>47</v>
+      </c>
+      <c r="H14" s="2"/>
+      <c r="L14"/>
+      <c r="M14" s="2"/>
+    </row>
+    <row r="15" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="E15" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G15" t="s">
+        <v>49</v>
+      </c>
+      <c r="H15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="M15" s="2"/>
+    </row>
+    <row r="16" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>69</v>
+      </c>
+      <c r="B16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G16" t="s">
+        <v>51</v>
+      </c>
+      <c r="H16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="M16" s="2"/>
+    </row>
+    <row r="17" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>69</v>
+      </c>
+      <c r="B17" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" t="s">
+        <v>53</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G17" t="s">
+        <v>53</v>
+      </c>
+      <c r="H17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="M17" s="2"/>
+    </row>
+    <row r="18" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>69</v>
+      </c>
+      <c r="B18" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G18" t="s">
+        <v>55</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="K18" s="2"/>
+      <c r="M18" s="2"/>
+    </row>
+    <row r="19" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>69</v>
+      </c>
+      <c r="B19" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" t="s">
+        <v>58</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G19" t="s">
+        <v>58</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="K19" s="2"/>
+      <c r="M19" s="2"/>
+    </row>
+    <row r="20" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>69</v>
+      </c>
+      <c r="B20" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G20" t="s">
+        <v>19</v>
+      </c>
+      <c r="K20" s="2"/>
+      <c r="M20" s="2"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E21" s="2"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E22" s="2"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E23" s="2"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E24" s="2"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E25" s="2"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E26" s="2"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E27" s="2"/>
+    </row>
+    <row r="39" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E39" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Correcties op Change waarden
En nieuwe all-translations
</commit_message>
<xml_diff>
--- a/zib2017-2020/mapping/excel/MedicatieToediening2.xlsx
+++ b/zib2017-2020/mapping/excel/MedicatieToediening2.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27425"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marcd\Dropbox\development\Zibtranslate\zib2017-2020\mapping\excel\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87A80F72-AB62-47F7-B68A-FD36CA0F850C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="translations" sheetId="1" r:id="rId1"/>
@@ -18,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">translations!$A$1:$O$20</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -199,6 +193,9 @@
     <t>groen: geen wijzigingen</t>
   </si>
   <si>
+    <t>oranje: minor change</t>
+  </si>
+  <si>
     <t>ZIB-911</t>
   </si>
   <si>
@@ -230,16 +227,13 @@
   </si>
   <si>
     <t>ZERO-TO-ONE TO ONE</t>
-  </si>
-  <si>
-    <t>oranje: minor change</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -304,7 +298,14 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFE403"/>
         </patternFill>
       </fill>
     </dxf>
@@ -318,34 +319,19 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFE403"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -383,7 +369,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -417,7 +403,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -452,10 +437,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -628,14 +612,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="40.7109375" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
@@ -644,7 +626,7 @@
     <col min="7" max="15" width="40.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -691,7 +673,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -711,7 +693,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -722,7 +704,7 @@
         <v>36</v>
       </c>
       <c r="E3" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="F3" t="s">
         <v>17</v>
@@ -731,28 +713,28 @@
         <v>36</v>
       </c>
       <c r="I3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="J3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="K3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="L3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="M3" t="s">
+        <v>66</v>
+      </c>
+      <c r="N3" t="s">
         <v>65</v>
       </c>
-      <c r="N3" t="s">
-        <v>64</v>
-      </c>
       <c r="O3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -772,7 +754,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -792,7 +774,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -812,7 +794,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -823,7 +805,7 @@
         <v>40</v>
       </c>
       <c r="E7" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="F7" t="s">
         <v>21</v>
@@ -832,28 +814,28 @@
         <v>40</v>
       </c>
       <c r="I7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="K7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="L7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="M7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="N7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="O7" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -873,7 +855,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -899,7 +881,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -919,7 +901,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -939,7 +921,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -959,7 +941,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -979,7 +961,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -999,7 +981,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -1019,7 +1001,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1039,7 +1021,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1059,7 +1041,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -1085,7 +1067,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -1111,7 +1093,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -1132,18 +1114,18 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:O20" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:O20"/>
   <conditionalFormatting sqref="E2:E20">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"groen: geen wijzigingen"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"geel: patch wijziging"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"oranje: minor change"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"rood: major change"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>